<commit_message>
added satellite receiver consumption
</commit_message>
<xml_diff>
--- a/data/consumption statistics/TV.xlsx
+++ b/data/consumption statistics/TV.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Uses/ hours</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>75'' Plasma</t>
+  </si>
+  <si>
+    <t>satellite receiver</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,15 +491,15 @@
         <v>1460</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C24" si="0">G3/1000</f>
+        <f t="shared" ref="C3:C19" si="0">G3/1000</f>
         <v>0.21</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D24" si="1">B3*C3</f>
+        <f t="shared" ref="D3:D18" si="1">B3*C3</f>
         <v>306.59999999999997</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E24" si="2">D3*0.17</f>
+        <f t="shared" ref="E3:E18" si="2">D3*0.17</f>
         <v>52.122</v>
       </c>
       <c r="G3">
@@ -837,15 +840,38 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f>B18*C18</f>
         <v>356.24</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f>D18*0.17</f>
         <v>60.560800000000008</v>
       </c>
       <c r="G18">
         <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>8760</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="D19">
+        <f>B19*C19</f>
+        <v>262.8</v>
+      </c>
+      <c r="E19">
+        <f>D19*0.17</f>
+        <v>44.676000000000002</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tv unit prices
</commit_message>
<xml_diff>
--- a/data/consumption statistics/TV.xlsx
+++ b/data/consumption statistics/TV.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Uses/ hours</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>satellite receiver</t>
+  </si>
+  <si>
+    <t>Cost (£)/pu (estimate)</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,7 +446,7 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:7" ht="42">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,6 +458,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -479,6 +485,9 @@
         <f>D2*0.17</f>
         <v>31.025000000000002</v>
       </c>
+      <c r="F2">
+        <v>280</v>
+      </c>
       <c r="G2">
         <v>125</v>
       </c>
@@ -495,12 +504,15 @@
         <v>0.21</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D18" si="1">B3*C3</f>
+        <f t="shared" ref="D3:D17" si="1">B3*C3</f>
         <v>306.59999999999997</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E18" si="2">D3*0.17</f>
+        <f t="shared" ref="E3:E17" si="2">D3*0.17</f>
         <v>52.122</v>
+      </c>
+      <c r="F3">
+        <v>420</v>
       </c>
       <c r="G3">
         <v>210</v>
@@ -525,6 +537,9 @@
         <f t="shared" si="2"/>
         <v>64.532000000000011</v>
       </c>
+      <c r="F4">
+        <v>900</v>
+      </c>
       <c r="G4">
         <v>260</v>
       </c>
@@ -548,6 +563,9 @@
         <f t="shared" si="2"/>
         <v>6.9496000000000011</v>
       </c>
+      <c r="F5">
+        <v>250</v>
+      </c>
       <c r="G5">
         <v>28</v>
       </c>
@@ -571,6 +589,9 @@
         <f t="shared" si="2"/>
         <v>9.4315999999999995</v>
       </c>
+      <c r="F6">
+        <v>320</v>
+      </c>
       <c r="G6">
         <v>38</v>
       </c>
@@ -594,6 +615,9 @@
         <f t="shared" si="2"/>
         <v>11.169</v>
       </c>
+      <c r="F7">
+        <v>380</v>
+      </c>
       <c r="G7">
         <v>45</v>
       </c>
@@ -617,6 +641,9 @@
         <f t="shared" si="2"/>
         <v>15.388400000000001</v>
       </c>
+      <c r="F8">
+        <v>700</v>
+      </c>
       <c r="G8">
         <v>62</v>
       </c>
@@ -640,6 +667,9 @@
         <f t="shared" si="2"/>
         <v>18.615000000000002</v>
       </c>
+      <c r="F9">
+        <v>1200</v>
+      </c>
       <c r="G9">
         <v>75</v>
       </c>
@@ -663,6 +693,9 @@
         <f t="shared" si="2"/>
         <v>21.8416</v>
       </c>
+      <c r="F10">
+        <v>2000</v>
+      </c>
       <c r="G10">
         <v>88</v>
       </c>
@@ -686,6 +719,9 @@
         <f t="shared" si="2"/>
         <v>24.82</v>
       </c>
+      <c r="F11">
+        <v>2500</v>
+      </c>
       <c r="G11">
         <v>100</v>
       </c>
@@ -709,6 +745,9 @@
         <f t="shared" si="2"/>
         <v>2.7302</v>
       </c>
+      <c r="F12">
+        <v>300</v>
+      </c>
       <c r="G12">
         <v>11</v>
       </c>
@@ -732,6 +771,9 @@
         <f t="shared" si="2"/>
         <v>10.672599999999999</v>
       </c>
+      <c r="F13">
+        <v>300</v>
+      </c>
       <c r="G13">
         <v>43</v>
       </c>
@@ -755,6 +797,9 @@
         <f t="shared" si="2"/>
         <v>16.133000000000003</v>
       </c>
+      <c r="F14">
+        <v>350</v>
+      </c>
       <c r="G14">
         <v>65</v>
       </c>
@@ -778,6 +823,9 @@
         <f t="shared" si="2"/>
         <v>29.535799999999998</v>
       </c>
+      <c r="F15">
+        <v>450</v>
+      </c>
       <c r="G15">
         <v>119</v>
       </c>
@@ -801,6 +849,9 @@
         <f t="shared" si="2"/>
         <v>40.456600000000009</v>
       </c>
+      <c r="F16">
+        <v>1000</v>
+      </c>
       <c r="G16">
         <v>163</v>
       </c>
@@ -824,6 +875,9 @@
         <f t="shared" si="2"/>
         <v>51.129200000000004</v>
       </c>
+      <c r="F17">
+        <v>2000</v>
+      </c>
       <c r="G17">
         <v>206</v>
       </c>
@@ -847,6 +901,9 @@
         <f>D18*0.17</f>
         <v>60.560800000000008</v>
       </c>
+      <c r="F18">
+        <v>2500</v>
+      </c>
       <c r="G18">
         <v>244</v>
       </c>
@@ -869,6 +926,9 @@
       <c r="E19">
         <f>D19*0.17</f>
         <v>44.676000000000002</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
       </c>
       <c r="G19">
         <v>30</v>

</xml_diff>